<commit_message>
Upload Y4_B2526_General_Surgery_checklist1758106406277_backup@backdoor.com.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_checklist1758106406277_backup@backdoor.com.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_checklist1758106406277_backup@backdoor.com.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\log_history\Imported_logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\Imported_logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5503A5E2-AE23-4B14-B347-116775E5F66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="3040" yWindow="580" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -273,7 +274,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -305,8 +309,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,29 +649,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="15.58203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -677,17 +682,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D2" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E2" t="s">
@@ -697,17 +702,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="C3" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D3" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E3" t="s">
@@ -717,17 +722,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D4" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E4" t="s">
@@ -737,17 +742,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D5" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E5" t="s">
@@ -757,17 +762,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D6" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E6" t="s">
@@ -777,17 +782,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D7" s="1">
+      <c r="C7" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D7" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E7" t="s">
@@ -797,17 +802,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D8" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E8" t="s">
@@ -817,17 +822,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D9" s="1">
+      <c r="C9" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D9" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E9" t="s">
@@ -837,17 +842,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D10" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E10" t="s">
@@ -857,17 +862,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D11" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E11" t="s">
@@ -877,17 +882,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D12" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E12" t="s">
@@ -897,17 +902,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D13" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E13" t="s">
@@ -917,17 +922,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D14" s="1">
+      <c r="C14" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D14" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E14" t="s">
@@ -937,17 +942,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="C15" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D15" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E15" t="s">
@@ -957,17 +962,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C16" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D16" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E16" t="s">
@@ -977,17 +982,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D17" s="1">
+      <c r="C17" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D17" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E17" t="s">
@@ -997,17 +1002,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="C18" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D18" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E18" t="s">
@@ -1017,17 +1022,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D19" s="1">
+      <c r="C19" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D19" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E19" t="s">
@@ -1037,17 +1042,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D20" s="1">
+      <c r="C20" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D20" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E20" t="s">
@@ -1057,17 +1062,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>28</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="C21" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D21" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E21" t="s">
@@ -1077,17 +1082,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="C22" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D22" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E22" t="s">
@@ -1097,17 +1102,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="C23" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D23" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E23" t="s">
@@ -1117,17 +1122,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="C24" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D24" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E24" t="s">
@@ -1137,17 +1142,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>32</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D25" s="1">
+      <c r="C25" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D25" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E25" t="s">
@@ -1157,17 +1162,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>33</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="C26" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D26" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E26" t="s">
@@ -1177,17 +1182,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="C27" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D27" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E27" t="s">
@@ -1197,17 +1202,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>36</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D28" s="1">
+      <c r="C28" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D28" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E28" t="s">
@@ -1217,17 +1222,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>37</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="C29" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D29" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E29" t="s">
@@ -1237,17 +1242,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D30" s="1">
+      <c r="C30" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D30" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E30" t="s">
@@ -1257,17 +1262,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>39</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D31" s="1">
+      <c r="C31" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D31" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E31" t="s">
@@ -1277,17 +1282,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>40</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D32" s="1">
+      <c r="C32" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D32" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E32" t="s">
@@ -1297,17 +1302,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>41</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D33" s="1">
+      <c r="C33" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D33" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E33" t="s">
@@ -1317,17 +1322,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>42</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D34" s="1">
+      <c r="C34" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D34" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E34" t="s">
@@ -1337,17 +1342,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>43</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D35" s="1">
+      <c r="C35" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D35" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E35" t="s">
@@ -1357,17 +1362,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>44</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D36" s="1">
+      <c r="C36" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D36" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E36" t="s">
@@ -1377,17 +1382,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>45</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D37" s="1">
+      <c r="C37" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D37" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E37" t="s">
@@ -1397,17 +1402,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>46</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D38" s="1">
+      <c r="C38" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D38" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E38" t="s">
@@ -1417,17 +1422,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>47</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D39" s="1">
+      <c r="C39" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D39" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E39" t="s">
@@ -1437,17 +1442,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>48</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D40" s="1">
+      <c r="C40" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D40" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E40" t="s">
@@ -1457,17 +1462,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>49</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D41" s="1">
+      <c r="C41" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D41" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E41" t="s">
@@ -1477,17 +1482,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>50</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D42" s="1">
+      <c r="C42" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D42" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E42" t="s">
@@ -1497,17 +1502,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>51</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D43" s="1">
+      <c r="C43" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D43" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E43" t="s">
@@ -1517,17 +1522,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>52</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D44" s="1">
+      <c r="C44" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D44" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E44" t="s">
@@ -1537,17 +1542,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>53</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D45" s="1">
+      <c r="C45" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D45" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E45" t="s">
@@ -1557,17 +1562,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>54</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D46" s="1">
+      <c r="C46" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D46" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E46" t="s">
@@ -1577,17 +1582,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>55</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D47" s="1">
+      <c r="C47" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D47" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E47" t="s">
@@ -1597,17 +1602,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>56</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D48" s="1">
+      <c r="C48" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D48" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E48" t="s">
@@ -1617,17 +1622,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>57</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D49" s="1">
+      <c r="C49" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D49" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E49" t="s">
@@ -1637,17 +1642,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>58</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D50" s="1">
+      <c r="C50" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D50" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E50" t="s">
@@ -1657,17 +1662,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>59</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
       </c>
-      <c r="C51" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D51" s="1">
+      <c r="C51" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D51" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E51" t="s">
@@ -1677,17 +1682,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>60</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D52" s="1">
+      <c r="C52" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D52" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E52" t="s">
@@ -1697,17 +1702,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>61</v>
       </c>
       <c r="B53" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D53" s="1">
+      <c r="C53" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D53" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E53" t="s">
@@ -1717,17 +1722,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>62</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D54" s="1">
+      <c r="C54" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D54" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E54" t="s">
@@ -1737,17 +1742,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>63</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
       </c>
-      <c r="C55" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D55" s="1">
+      <c r="C55" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D55" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E55" t="s">
@@ -1757,17 +1762,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>64</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D56" s="1">
+      <c r="C56" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D56" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E56" t="s">
@@ -1777,17 +1782,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>65</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
-      <c r="C57" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D57" s="1">
+      <c r="C57" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D57" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E57" t="s">
@@ -1797,17 +1802,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>66</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
-      <c r="C58" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D58" s="1">
+      <c r="C58" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D58" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E58" t="s">
@@ -1817,17 +1822,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>67</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
       </c>
-      <c r="C59" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D59" s="1">
+      <c r="C59" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D59" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E59" t="s">
@@ -1837,17 +1842,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>68</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
       </c>
-      <c r="C60" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D60" s="1">
+      <c r="C60" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D60" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E60" t="s">
@@ -1857,17 +1862,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>69</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
       </c>
-      <c r="C61" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D61" s="1">
+      <c r="C61" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D61" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E61" t="s">
@@ -1877,17 +1882,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>70</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
       </c>
-      <c r="C62" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D62" s="1">
+      <c r="C62" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D62" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E62" t="s">
@@ -1897,17 +1902,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>71</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
       </c>
-      <c r="C63" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D63" s="1">
+      <c r="C63" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D63" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E63" t="s">
@@ -1917,17 +1922,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>72</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
       </c>
-      <c r="C64" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D64" s="1">
+      <c r="C64" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D64" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E64" t="s">
@@ -1937,17 +1942,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>73</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D65" s="1">
+      <c r="C65" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D65" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E65" t="s">
@@ -1957,17 +1962,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>74</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D66" s="1">
+      <c r="C66" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D66" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E66" t="s">
@@ -1977,17 +1982,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>75</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D67" s="1">
+      <c r="C67" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D67" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E67" t="s">
@@ -1997,17 +2002,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>76</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
       </c>
-      <c r="C68" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D68" s="1">
+      <c r="C68" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D68" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E68" t="s">
@@ -2017,17 +2022,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>77</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D69" s="1">
+      <c r="C69" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D69" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E69" t="s">
@@ -2037,17 +2042,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>78</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
       </c>
-      <c r="C70" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D70" s="1">
+      <c r="C70" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D70" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E70" t="s">
@@ -2057,17 +2062,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>79</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
       </c>
-      <c r="C71" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D71" s="1">
+      <c r="C71" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D71" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E71" t="s">
@@ -2077,17 +2082,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>80</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
       </c>
-      <c r="C72" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D72" s="1">
+      <c r="C72" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D72" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E72" t="s">
@@ -2097,17 +2102,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>81</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
       </c>
-      <c r="C73" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D73" s="1">
+      <c r="C73" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D73" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E73" t="s">
@@ -2117,17 +2122,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>82</v>
       </c>
       <c r="B74" t="s">
         <v>7</v>
       </c>
-      <c r="C74" s="2">
-        <v>45878</v>
-      </c>
-      <c r="D74" s="1">
+      <c r="C74" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D74" s="2">
         <v>0.49553240740740739</v>
       </c>
       <c r="E74" t="s">

</xml_diff>